<commit_message>
put in more real detail
Made it look more like what the real rat data files would look like for
the excel file, and started integrating changes to read in excel file
into python
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -13,6 +13,38 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+  <si>
+    <t>07.08.16</t>
+  </si>
+  <si>
+    <t>T-0706</t>
+  </si>
+  <si>
+    <t>R158M</t>
+  </si>
+  <si>
+    <t>R185U</t>
+  </si>
+  <si>
+    <t>R165M</t>
+  </si>
+  <si>
+    <t>R170U</t>
+  </si>
+  <si>
+    <t>R173M</t>
+  </si>
+  <si>
+    <t>R176U</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -64,6 +96,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -367,363 +403,393 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>458</v>
-      </c>
-      <c r="C1" s="1">
-        <v>428</v>
-      </c>
-      <c r="D1" s="1">
-        <v>541</v>
-      </c>
-      <c r="E1" s="1">
-        <v>413</v>
-      </c>
-      <c r="F1" s="1">
-        <v>428</v>
-      </c>
-      <c r="G1" s="3">
-        <v>480</v>
-      </c>
-      <c r="H1" s="1">
-        <f>AVERAGE(B1:G1)</f>
-        <v>458</v>
-      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
-        <v>380</v>
-      </c>
-      <c r="C2" s="1">
-        <v>318</v>
-      </c>
-      <c r="D2" s="1">
-        <v>331</v>
-      </c>
-      <c r="E2" s="1">
-        <v>355</v>
-      </c>
-      <c r="F2" s="1">
-        <v>346</v>
-      </c>
-      <c r="G2" s="3">
-        <v>254</v>
-      </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:H13" si="0">AVERAGE(B2:G2)</f>
-        <v>330.66666666666669</v>
-      </c>
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2">
-        <v>317</v>
-      </c>
-      <c r="C3" s="1">
-        <v>250</v>
-      </c>
-      <c r="D3" s="1">
-        <v>321</v>
-      </c>
-      <c r="E3" s="1">
-        <v>298</v>
-      </c>
-      <c r="F3" s="1">
-        <v>267</v>
-      </c>
-      <c r="G3" s="3">
-        <v>268</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" si="0"/>
-        <v>286.83333333333331</v>
-      </c>
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>316</v>
+        <v>458</v>
       </c>
       <c r="C4" s="1">
-        <v>198</v>
+        <v>428</v>
       </c>
       <c r="D4" s="1">
-        <v>287</v>
+        <v>541</v>
       </c>
       <c r="E4" s="1">
-        <v>236</v>
+        <v>413</v>
       </c>
       <c r="F4" s="1">
-        <v>249</v>
+        <v>428</v>
       </c>
       <c r="G4" s="3">
-        <v>204</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="0"/>
-        <v>248.33333333333334</v>
-      </c>
+        <v>480</v>
+      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
-        <v>251</v>
+        <v>380</v>
       </c>
       <c r="C5" s="1">
-        <v>169</v>
+        <v>318</v>
       </c>
       <c r="D5" s="1">
-        <v>291</v>
+        <v>331</v>
       </c>
       <c r="E5" s="1">
-        <v>188</v>
+        <v>355</v>
       </c>
       <c r="F5" s="1">
-        <v>232</v>
+        <v>346</v>
       </c>
       <c r="G5" s="3">
-        <v>214</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="0"/>
-        <v>224.16666666666666</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>262</v>
+        <v>317</v>
       </c>
       <c r="C6" s="1">
-        <v>164</v>
+        <v>250</v>
       </c>
       <c r="D6" s="1">
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="E6" s="1">
-        <v>164</v>
+        <v>298</v>
       </c>
       <c r="F6" s="1">
-        <v>183</v>
+        <v>267</v>
       </c>
       <c r="G6" s="3">
-        <v>201</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="0"/>
-        <v>208.66666666666666</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2">
-        <v>241</v>
+        <v>316</v>
       </c>
       <c r="C7" s="1">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="D7" s="1">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="E7" s="1">
-        <v>154</v>
+        <v>236</v>
       </c>
       <c r="F7" s="1">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="G7" s="3">
-        <v>144</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="0"/>
-        <v>187.33333333333334</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="C8" s="1">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D8" s="1">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E8" s="1">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="F8" s="1">
-        <v>169</v>
+        <v>232</v>
       </c>
       <c r="G8" s="3">
-        <v>148</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="0"/>
-        <v>193.16666666666666</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="C9" s="1">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="D9" s="1">
-        <v>339</v>
+        <v>278</v>
       </c>
       <c r="E9" s="1">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F9" s="1">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G9" s="3">
-        <v>166</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="0"/>
-        <v>223.83333333333334</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2">
-        <v>296</v>
+        <v>241</v>
       </c>
       <c r="C10" s="1">
-        <v>236</v>
+        <v>137</v>
       </c>
       <c r="D10" s="1">
-        <v>336</v>
+        <v>266</v>
       </c>
       <c r="E10" s="1">
-        <v>215</v>
+        <v>154</v>
       </c>
       <c r="F10" s="1">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="G10" s="3">
-        <v>188</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="0"/>
-        <v>248.33333333333334</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="B11" s="2">
-        <v>334</v>
+        <v>239</v>
       </c>
       <c r="C11" s="1">
-        <v>266</v>
+        <v>167</v>
       </c>
       <c r="D11" s="1">
-        <v>335</v>
+        <v>296</v>
       </c>
       <c r="E11" s="1">
-        <v>244</v>
+        <v>140</v>
       </c>
       <c r="F11" s="1">
-        <v>236</v>
+        <v>169</v>
       </c>
       <c r="G11" s="3">
-        <v>193</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="0"/>
-        <v>268</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="B12" s="2">
-        <v>342</v>
+        <v>281</v>
       </c>
       <c r="C12" s="1">
-        <v>277</v>
+        <v>199</v>
       </c>
       <c r="D12" s="1">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="E12" s="1">
-        <v>279</v>
+        <v>162</v>
       </c>
       <c r="F12" s="1">
-        <v>261</v>
+        <v>196</v>
       </c>
       <c r="G12" s="3">
-        <v>249</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="0"/>
-        <v>294</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <v>120</v>
+      </c>
+      <c r="B13" s="2">
+        <v>296</v>
+      </c>
+      <c r="C13" s="1">
+        <v>236</v>
+      </c>
+      <c r="D13" s="1">
+        <v>336</v>
+      </c>
+      <c r="E13" s="1">
+        <v>215</v>
+      </c>
+      <c r="F13" s="1">
+        <v>219</v>
+      </c>
+      <c r="G13" s="3">
+        <v>188</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>150</v>
+      </c>
+      <c r="B14" s="2">
+        <v>334</v>
+      </c>
+      <c r="C14" s="1">
+        <v>266</v>
+      </c>
+      <c r="D14" s="1">
+        <v>335</v>
+      </c>
+      <c r="E14" s="1">
+        <v>244</v>
+      </c>
+      <c r="F14" s="1">
+        <v>236</v>
+      </c>
+      <c r="G14" s="3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>180</v>
+      </c>
+      <c r="B15" s="2">
+        <v>342</v>
+      </c>
+      <c r="C15" s="1">
+        <v>277</v>
+      </c>
+      <c r="D15" s="1">
+        <v>356</v>
+      </c>
+      <c r="E15" s="1">
+        <v>279</v>
+      </c>
+      <c r="F15" s="1">
+        <v>261</v>
+      </c>
+      <c r="G15" s="3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>240</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B16" s="2">
         <v>298</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C16" s="1">
         <v>312</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D16" s="1">
         <v>388</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E16" s="1">
         <v>325</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F16" s="1">
         <v>308</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G16" s="3">
         <v>300</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" si="0"/>
-        <v>321.83333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally Read in Excel file!
read excel file in to the code and am now calculating mean of a single
TA. Not sure if this needs to be scaled up or not. Will get this piece
working and revisit.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="12855"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
   <si>
     <t>07.08.16</t>
   </si>
@@ -403,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -433,9 +433,56 @@
       <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1">
+        <v>30</v>
+      </c>
+      <c r="O1" s="1">
+        <v>40</v>
+      </c>
+      <c r="P1" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>60</v>
+      </c>
+      <c r="R1" s="1">
+        <v>80</v>
+      </c>
+      <c r="S1" s="1">
+        <v>100</v>
+      </c>
+      <c r="T1" s="1">
+        <v>120</v>
+      </c>
+      <c r="U1" s="1">
+        <v>150</v>
+      </c>
+      <c r="V1" s="1">
+        <v>180</v>
+      </c>
+      <c r="W1" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -457,9 +504,56 @@
       <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>458</v>
+      </c>
+      <c r="L2" s="2">
+        <v>380</v>
+      </c>
+      <c r="M2" s="2">
+        <v>317</v>
+      </c>
+      <c r="N2" s="2">
+        <v>316</v>
+      </c>
+      <c r="O2" s="2">
+        <v>251</v>
+      </c>
+      <c r="P2" s="2">
+        <v>262</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>241</v>
+      </c>
+      <c r="R2" s="2">
+        <v>239</v>
+      </c>
+      <c r="S2" s="2">
+        <v>281</v>
+      </c>
+      <c r="T2" s="2">
+        <v>296</v>
+      </c>
+      <c r="U2" s="2">
+        <v>334</v>
+      </c>
+      <c r="V2" s="2">
+        <v>342</v>
+      </c>
+      <c r="W2" s="2">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -481,9 +575,56 @@
       <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>428</v>
+      </c>
+      <c r="L3" s="1">
+        <v>318</v>
+      </c>
+      <c r="M3" s="1">
+        <v>250</v>
+      </c>
+      <c r="N3" s="1">
+        <v>198</v>
+      </c>
+      <c r="O3" s="1">
+        <v>169</v>
+      </c>
+      <c r="P3" s="1">
+        <v>164</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>137</v>
+      </c>
+      <c r="R3" s="1">
+        <v>167</v>
+      </c>
+      <c r="S3" s="1">
+        <v>199</v>
+      </c>
+      <c r="T3" s="1">
+        <v>236</v>
+      </c>
+      <c r="U3" s="1">
+        <v>266</v>
+      </c>
+      <c r="V3" s="1">
+        <v>277</v>
+      </c>
+      <c r="W3" s="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -505,9 +646,56 @@
       <c r="G4" s="3">
         <v>480</v>
       </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>541</v>
+      </c>
+      <c r="L4" s="1">
+        <v>331</v>
+      </c>
+      <c r="M4" s="1">
+        <v>321</v>
+      </c>
+      <c r="N4" s="1">
+        <v>287</v>
+      </c>
+      <c r="O4" s="1">
+        <v>291</v>
+      </c>
+      <c r="P4" s="1">
+        <v>278</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>266</v>
+      </c>
+      <c r="R4" s="1">
+        <v>296</v>
+      </c>
+      <c r="S4" s="1">
+        <v>339</v>
+      </c>
+      <c r="T4" s="1">
+        <v>336</v>
+      </c>
+      <c r="U4" s="1">
+        <v>335</v>
+      </c>
+      <c r="V4" s="1">
+        <v>356</v>
+      </c>
+      <c r="W4" s="1">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -529,9 +717,56 @@
       <c r="G5" s="3">
         <v>254</v>
       </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>413</v>
+      </c>
+      <c r="L5" s="1">
+        <v>355</v>
+      </c>
+      <c r="M5" s="1">
+        <v>298</v>
+      </c>
+      <c r="N5" s="1">
+        <v>236</v>
+      </c>
+      <c r="O5" s="1">
+        <v>188</v>
+      </c>
+      <c r="P5" s="1">
+        <v>164</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>154</v>
+      </c>
+      <c r="R5" s="1">
+        <v>140</v>
+      </c>
+      <c r="S5" s="1">
+        <v>162</v>
+      </c>
+      <c r="T5" s="1">
+        <v>215</v>
+      </c>
+      <c r="U5" s="1">
+        <v>244</v>
+      </c>
+      <c r="V5" s="1">
+        <v>279</v>
+      </c>
+      <c r="W5" s="1">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>20</v>
       </c>
@@ -553,9 +788,56 @@
       <c r="G6" s="3">
         <v>268</v>
       </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>428</v>
+      </c>
+      <c r="L6" s="1">
+        <v>346</v>
+      </c>
+      <c r="M6" s="1">
+        <v>267</v>
+      </c>
+      <c r="N6" s="1">
+        <v>249</v>
+      </c>
+      <c r="O6" s="1">
+        <v>232</v>
+      </c>
+      <c r="P6" s="1">
+        <v>183</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>182</v>
+      </c>
+      <c r="R6" s="1">
+        <v>169</v>
+      </c>
+      <c r="S6" s="1">
+        <v>196</v>
+      </c>
+      <c r="T6" s="1">
+        <v>219</v>
+      </c>
+      <c r="U6" s="1">
+        <v>236</v>
+      </c>
+      <c r="V6" s="1">
+        <v>261</v>
+      </c>
+      <c r="W6" s="1">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>30</v>
       </c>
@@ -577,9 +859,56 @@
       <c r="G7" s="3">
         <v>204</v>
       </c>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="3">
+        <v>480</v>
+      </c>
+      <c r="L7" s="3">
+        <v>254</v>
+      </c>
+      <c r="M7" s="3">
+        <v>268</v>
+      </c>
+      <c r="N7" s="3">
+        <v>204</v>
+      </c>
+      <c r="O7" s="3">
+        <v>214</v>
+      </c>
+      <c r="P7" s="3">
+        <v>201</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>144</v>
+      </c>
+      <c r="R7" s="3">
+        <v>148</v>
+      </c>
+      <c r="S7" s="3">
+        <v>166</v>
+      </c>
+      <c r="T7" s="3">
+        <v>188</v>
+      </c>
+      <c r="U7" s="3">
+        <v>193</v>
+      </c>
+      <c r="V7" s="3">
+        <v>249</v>
+      </c>
+      <c r="W7" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>40</v>
       </c>
@@ -603,7 +932,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>50</v>
       </c>
@@ -627,7 +956,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>60</v>
       </c>
@@ -651,7 +980,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>80</v>
       </c>
@@ -675,7 +1004,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -699,7 +1028,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>120</v>
       </c>
@@ -723,7 +1052,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>150</v>
       </c>
@@ -746,7 +1075,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>180</v>
       </c>
@@ -769,7 +1098,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>240</v>
       </c>

</xml_diff>